<commit_message>
Domain y dto Compañia
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/medic/MedicoFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/medic/MedicoFormulario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\API\Service.Catalog\wwwroot\layout\excel\medic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0A796D-D912-429E-BF8A-C92F54360ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D00D52-67EE-4BD0-9853-8F4C0E131AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
@@ -173,10 +173,10 @@
     <t>Ciudad</t>
   </si>
   <si>
-    <t>{{Medico.Estado}}</t>
-  </si>
-  <si>
-    <t>{{Medico.Ciudad}}</t>
+    <t>{{Medico.EstadoId}}</t>
+  </si>
+  <si>
+    <t>{{Medico.CiudadId}}</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>